<commit_message>
changed assignment file and added IDE and PL
</commit_message>
<xml_diff>
--- a/Week4. Correct requirements and life cycle/Assignment.xlsx
+++ b/Week4. Correct requirements and life cycle/Assignment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
   <si>
     <t>#</t>
   </si>
@@ -134,12 +134,24 @@
   </si>
   <si>
     <t>Как я понял, препод никак не может понять, как мы будем проверять задачи. Подробно расписать, что и как</t>
+  </si>
+  <si>
+    <t>Отметка о выполении</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -169,10 +181,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,9 +510,11 @@
     <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="115.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -504,8 +527,14 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -515,11 +544,14 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -529,9 +561,12 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -544,8 +579,11 @@
       <c r="D4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -558,8 +596,11 @@
       <c r="D5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -572,8 +613,11 @@
       <c r="D6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -586,8 +630,11 @@
       <c r="D7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -600,8 +647,11 @@
       <c r="D8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -611,8 +661,11 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -622,8 +675,11 @@
       <c r="C10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -636,8 +692,14 @@
       <c r="D11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3">
+        <v>42273.833333333336</v>
+      </c>
+      <c r="F11" s="4">
+        <v>42272.979166666664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -650,8 +712,14 @@
       <c r="D12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="3">
+        <v>42273.833333333336</v>
+      </c>
+      <c r="F12" s="4">
+        <v>42272.979166666664</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -664,8 +732,11 @@
       <c r="D13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="3">
+        <v>42273.833333333336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -675,8 +746,11 @@
       <c r="C14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="3">
+        <v>42274.958333333336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -686,8 +760,14 @@
       <c r="C15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="3">
+        <v>42270.833333333336</v>
+      </c>
+      <c r="F15" s="4">
+        <v>42269.083333333336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -696,6 +776,9 @@
       </c>
       <c r="C16" t="s">
         <v>30</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final assignment and week results
</commit_message>
<xml_diff>
--- a/Week4. Correct requirements and life cycle/Assignment.xlsx
+++ b/Week4. Correct requirements and life cycle/Assignment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>#</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Продлено до 27.09.15 9:00</t>
+  </si>
+  <si>
+    <t>Не были присланы вовремя все файлы от второй группы</t>
   </si>
 </sst>
 </file>
@@ -559,7 +562,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,7 +637,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -648,6 +651,9 @@
       </c>
       <c r="E4" s="2">
         <v>42273.833333333336</v>
+      </c>
+      <c r="F4" s="3">
+        <v>42274.916666666664</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -711,7 +717,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -725,6 +731,9 @@
       </c>
       <c r="E8" s="2">
         <v>42273.833333333336</v>
+      </c>
+      <c r="F8" s="3">
+        <v>42274.083333333336</v>
       </c>
       <c r="G8" t="s">
         <v>44</v>
@@ -743,12 +752,15 @@
       <c r="E9" s="2">
         <v>42273.833333333336</v>
       </c>
+      <c r="F9" s="3">
+        <v>42274.083333333336</v>
+      </c>
       <c r="G9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -759,6 +771,9 @@
       </c>
       <c r="E10" s="2">
         <v>42273.833333333336</v>
+      </c>
+      <c r="F10" s="3">
+        <v>42274.083333333336</v>
       </c>
       <c r="G10" t="s">
         <v>44</v>
@@ -825,7 +840,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -836,6 +851,12 @@
       </c>
       <c r="E14" s="2">
         <v>42274.958333333336</v>
+      </c>
+      <c r="F14" s="3">
+        <v>42274.957638888889</v>
+      </c>
+      <c r="G14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>